<commit_message>
added HIT 923 to 926
</commit_message>
<xml_diff>
--- a/corpus_info.xlsx
+++ b/corpus_info.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="680" yWindow="460" windowWidth="28320" windowHeight="17320" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="1260" yWindow="460" windowWidth="26020" windowHeight="16920" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="amt_902_096" sheetId="5" r:id="rId1"/>
-    <sheet name="amt_907_915_tk" sheetId="4" r:id="rId2"/>
-    <sheet name="amt_916_919_tk" sheetId="1" r:id="rId3"/>
-    <sheet name="amt_920_922_tk" sheetId="2" r:id="rId4"/>
+    <sheet name="amt_916_919_tk" sheetId="1" r:id="rId2"/>
+    <sheet name="amt_920_922_tk" sheetId="2" r:id="rId3"/>
+    <sheet name="amt_907_915_tk" sheetId="4" r:id="rId4"/>
+    <sheet name="amt_923_tk" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="423">
   <si>
     <t>entryCode</t>
   </si>
@@ -1044,13 +1045,268 @@
   </si>
   <si>
     <t>tuker.index</t>
+  </si>
+  <si>
+    <t>AS48VQ5416HWN</t>
+  </si>
+  <si>
+    <t>a07d04518afeda11f7583f6ab1f9cffa</t>
+  </si>
+  <si>
+    <t>A3JXSXBWYBD5M6</t>
+  </si>
+  <si>
+    <t>e2b9eb967216d791254fabada59d7263</t>
+  </si>
+  <si>
+    <t>A31UXXZVI3U4E2</t>
+  </si>
+  <si>
+    <t>cbd157fa9d450d7e9ca762c0069d25d8</t>
+  </si>
+  <si>
+    <t>AL0IT4RSPIWGK</t>
+  </si>
+  <si>
+    <t>4f2505355cca44dc815d64187ec00d30</t>
+  </si>
+  <si>
+    <t>ATX360P459MCZ</t>
+  </si>
+  <si>
+    <t>e106ab53b60fd4eb4ab1b7af3bc25a35</t>
+  </si>
+  <si>
+    <t>A1F9KLZGHE9DTA</t>
+  </si>
+  <si>
+    <t>5c638ec5499a150f6d21c734f3888f8a</t>
+  </si>
+  <si>
+    <t>ASHLFU48WG2CH</t>
+  </si>
+  <si>
+    <t>19faed6304df40e4f0b9255819e1abbf</t>
+  </si>
+  <si>
+    <t>A2BNOEYZ3VRW2R</t>
+  </si>
+  <si>
+    <t>ba78b475138be28e768e2626417cbaaa</t>
+  </si>
+  <si>
+    <t>A25M8E1A9XVR5A</t>
+  </si>
+  <si>
+    <t>fd9d861914d43203dac70468d111377e</t>
+  </si>
+  <si>
+    <t>A1BNGJBEWJS8WE</t>
+  </si>
+  <si>
+    <t>f749c70ebe181739d99adc52a383f2ba</t>
+  </si>
+  <si>
+    <t>A2VD133723IZR8</t>
+  </si>
+  <si>
+    <t>e432130a9281459a9eb2db95824d3e68</t>
+  </si>
+  <si>
+    <t>A1ISETF211O6JL</t>
+  </si>
+  <si>
+    <t>e213f8c31ae785b0a2616ea57a094355</t>
+  </si>
+  <si>
+    <t>A3UE4L8VJXY3PE</t>
+  </si>
+  <si>
+    <t>e1d1fdb09371f3201b9c701ebfa5bd5a</t>
+  </si>
+  <si>
+    <t>A2B1X24DLNGXJ3</t>
+  </si>
+  <si>
+    <t>dd11cd4d18fdce2773999a0b938d7a7a</t>
+  </si>
+  <si>
+    <t>A24APYGPICROST</t>
+  </si>
+  <si>
+    <t>d0a820a941ae2524a5bddada2d3e8c8e</t>
+  </si>
+  <si>
+    <t>A3BHWGNQUVMEKU</t>
+  </si>
+  <si>
+    <t>cb423ef44707061e91451efcb8209246</t>
+  </si>
+  <si>
+    <t>AC5UD8N187QD6</t>
+  </si>
+  <si>
+    <t>c5d92b38d3c7f7dcb567a4dccc0b46c9</t>
+  </si>
+  <si>
+    <t>A26TTXM6B7771S</t>
+  </si>
+  <si>
+    <t>c4f6d3f5d837c4faf5454f784396d482</t>
+  </si>
+  <si>
+    <t>A1MDTLVYHRI62J</t>
+  </si>
+  <si>
+    <t>bc7d328fe052fc0cfec83f78ded29a2d</t>
+  </si>
+  <si>
+    <t>A2L7S6RZOZ6NM9</t>
+  </si>
+  <si>
+    <t>bb4da9ba86583af0938eb9a61e99cb2a</t>
+  </si>
+  <si>
+    <t>A3NWDC5NASS71Y</t>
+  </si>
+  <si>
+    <t>b10560f945e192f8bea6798a843cb276</t>
+  </si>
+  <si>
+    <t>A30MJ6JMKVNOGS</t>
+  </si>
+  <si>
+    <t>a20b65d421c479ad77036b41a446a568</t>
+  </si>
+  <si>
+    <t>A1OQ3KL56KMQSU</t>
+  </si>
+  <si>
+    <t>958fa74020c6ec872c0da2669a237995</t>
+  </si>
+  <si>
+    <t>AYSHA8Y5BOFFF</t>
+  </si>
+  <si>
+    <t>9274b79d04b59915b5e6901d95ae402f</t>
+  </si>
+  <si>
+    <t>A36GGN5JFG7LQ6</t>
+  </si>
+  <si>
+    <t>8f818909013d8d4e59a4530b2ee321d9</t>
+  </si>
+  <si>
+    <t>80c27fb8a30a21f2ff0d0a2ce2d12d59</t>
+  </si>
+  <si>
+    <t>A1PUHCEBSOWETV</t>
+  </si>
+  <si>
+    <t>72332419bd7bc52f7e1717dd700a0001</t>
+  </si>
+  <si>
+    <t>AIYJ5S5A9OR2I</t>
+  </si>
+  <si>
+    <t>719c5544010e8f5e30df534550a23666</t>
+  </si>
+  <si>
+    <t>A2PT8D2MIYQPDD</t>
+  </si>
+  <si>
+    <t>6a2743ae522c26160e2a5a7216475b83</t>
+  </si>
+  <si>
+    <t>AMYURTQIMAC8T</t>
+  </si>
+  <si>
+    <t>651ad7462dd394a9477498bc799d0481</t>
+  </si>
+  <si>
+    <t>A2M9MD6AHXVT54</t>
+  </si>
+  <si>
+    <t>469dc4e4f4edceef87a28a5d2380826f</t>
+  </si>
+  <si>
+    <t>A2WYCY1FMQOD5F</t>
+  </si>
+  <si>
+    <t>45b114165c29b1e2977a1daba62d7dc2</t>
+  </si>
+  <si>
+    <t>A3R7VRRBNH4T2Z</t>
+  </si>
+  <si>
+    <t>2fb511a147d4da2d44f34ace2049950e</t>
+  </si>
+  <si>
+    <t>A1GFLFS4YKCTLU</t>
+  </si>
+  <si>
+    <t>2ab58e1bce4c879b49642165350073a8</t>
+  </si>
+  <si>
+    <t>A2SMQ7NHIWTQMA</t>
+  </si>
+  <si>
+    <t>25d26396e4c8b7a75bc2f8e9f87016cf</t>
+  </si>
+  <si>
+    <t>A2XG3FPY0UDZIJ</t>
+  </si>
+  <si>
+    <t>25016252adb22ba9b2710f8629bbb3c8</t>
+  </si>
+  <si>
+    <t>A1OTFSUC6Y1J10</t>
+  </si>
+  <si>
+    <t>1130e8945f9b79edfa4ee6f50b3e3780</t>
+  </si>
+  <si>
+    <t>A2UYHVYUOSEVGS</t>
+  </si>
+  <si>
+    <t>0c44f8c8dffb4c623c53b613fd6debcc</t>
+  </si>
+  <si>
+    <t>A1J4N2SE30LCUH</t>
+  </si>
+  <si>
+    <t>0601c378f854e8931569d0d277736a7f</t>
+  </si>
+  <si>
+    <t>A21SIPO89DP66I</t>
+  </si>
+  <si>
+    <t>03daf1413c588d606c8428150a48dcb6</t>
+  </si>
+  <si>
+    <t>A367ZURE8LUTJV</t>
+  </si>
+  <si>
+    <t>035641ffc501e7e65469f492a2d0631c</t>
+  </si>
+  <si>
+    <t>turker.Index</t>
+  </si>
+  <si>
+    <t>video cannot be played</t>
+  </si>
+  <si>
+    <t>video quality is too low.</t>
+  </si>
+  <si>
+    <t>A good example; sitting pose is very like in a real interview</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1065,6 +1321,23 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1105,7 +1378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1113,6 +1386,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1788,856 +2064,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G42"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="33.83203125" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>285</v>
-      </c>
-      <c r="B2">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>284</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>283</v>
-      </c>
-      <c r="B3">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>282</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>281</v>
-      </c>
-      <c r="B4">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>280</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>279</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>278</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>286</v>
-      </c>
-      <c r="G5">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>277</v>
-      </c>
-      <c r="B6">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>276</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>275</v>
-      </c>
-      <c r="B7">
-        <v>8</v>
-      </c>
-      <c r="C7">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>274</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>273</v>
-      </c>
-      <c r="B8">
-        <v>8</v>
-      </c>
-      <c r="C8">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>272</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>271</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>270</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>269</v>
-      </c>
-      <c r="B10">
-        <v>8</v>
-      </c>
-      <c r="C10">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>268</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>267</v>
-      </c>
-      <c r="B11">
-        <v>8</v>
-      </c>
-      <c r="C11">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>266</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>265</v>
-      </c>
-      <c r="B12">
-        <v>8</v>
-      </c>
-      <c r="C12">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>264</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>263</v>
-      </c>
-      <c r="B13">
-        <v>8</v>
-      </c>
-      <c r="C13">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>262</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B14">
-        <v>8</v>
-      </c>
-      <c r="C14">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
-        <v>260</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>259</v>
-      </c>
-      <c r="B15">
-        <v>8</v>
-      </c>
-      <c r="C15">
-        <v>8</v>
-      </c>
-      <c r="D15" t="s">
-        <v>258</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>257</v>
-      </c>
-      <c r="B16">
-        <v>8</v>
-      </c>
-      <c r="C16">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>256</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>255</v>
-      </c>
-      <c r="B17">
-        <v>8</v>
-      </c>
-      <c r="C17">
-        <v>8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>254</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>253</v>
-      </c>
-      <c r="B18">
-        <v>8</v>
-      </c>
-      <c r="C18">
-        <v>8</v>
-      </c>
-      <c r="D18" t="s">
-        <v>252</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>251</v>
-      </c>
-      <c r="B19">
-        <v>8</v>
-      </c>
-      <c r="C19">
-        <v>8</v>
-      </c>
-      <c r="D19" t="s">
-        <v>250</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>249</v>
-      </c>
-      <c r="B20">
-        <v>8</v>
-      </c>
-      <c r="C20">
-        <v>8</v>
-      </c>
-      <c r="D20" t="s">
-        <v>248</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>247</v>
-      </c>
-      <c r="B21">
-        <v>8</v>
-      </c>
-      <c r="C21">
-        <v>8</v>
-      </c>
-      <c r="D21" t="s">
-        <v>246</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>245</v>
-      </c>
-      <c r="B22">
-        <v>8</v>
-      </c>
-      <c r="C22">
-        <v>8</v>
-      </c>
-      <c r="D22" t="s">
-        <v>244</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>243</v>
-      </c>
-      <c r="B23">
-        <v>8</v>
-      </c>
-      <c r="C23">
-        <v>8</v>
-      </c>
-      <c r="D23" t="s">
-        <v>242</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="G23">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>241</v>
-      </c>
-      <c r="B24">
-        <v>8</v>
-      </c>
-      <c r="C24">
-        <v>8</v>
-      </c>
-      <c r="D24" t="s">
-        <v>240</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="G24">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>239</v>
-      </c>
-      <c r="B25">
-        <v>8</v>
-      </c>
-      <c r="C25">
-        <v>8</v>
-      </c>
-      <c r="D25" t="s">
-        <v>238</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>237</v>
-      </c>
-      <c r="B26">
-        <v>8</v>
-      </c>
-      <c r="C26">
-        <v>8</v>
-      </c>
-      <c r="D26" t="s">
-        <v>236</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>235</v>
-      </c>
-      <c r="B27">
-        <v>8</v>
-      </c>
-      <c r="C27">
-        <v>8</v>
-      </c>
-      <c r="D27" t="s">
-        <v>234</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>233</v>
-      </c>
-      <c r="B28">
-        <v>8</v>
-      </c>
-      <c r="C28">
-        <v>8</v>
-      </c>
-      <c r="D28" t="s">
-        <v>232</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="G28">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>231</v>
-      </c>
-      <c r="B29">
-        <v>8</v>
-      </c>
-      <c r="C29">
-        <v>8</v>
-      </c>
-      <c r="D29" t="s">
-        <v>230</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="G29">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>229</v>
-      </c>
-      <c r="B30">
-        <v>8</v>
-      </c>
-      <c r="C30">
-        <v>8</v>
-      </c>
-      <c r="D30" t="s">
-        <v>228</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-      <c r="G30">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>227</v>
-      </c>
-      <c r="B31">
-        <v>8</v>
-      </c>
-      <c r="C31">
-        <v>8</v>
-      </c>
-      <c r="D31" t="s">
-        <v>226</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-      <c r="G31">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>225</v>
-      </c>
-      <c r="B32">
-        <v>8</v>
-      </c>
-      <c r="C32">
-        <v>8</v>
-      </c>
-      <c r="D32" t="s">
-        <v>224</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-      <c r="G32">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>223</v>
-      </c>
-      <c r="B33">
-        <v>8</v>
-      </c>
-      <c r="C33">
-        <v>8</v>
-      </c>
-      <c r="D33" t="s">
-        <v>222</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="G33">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>221</v>
-      </c>
-      <c r="B34">
-        <v>8</v>
-      </c>
-      <c r="C34">
-        <v>8</v>
-      </c>
-      <c r="D34" t="s">
-        <v>220</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="G34">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>219</v>
-      </c>
-      <c r="B35">
-        <v>8</v>
-      </c>
-      <c r="C35">
-        <v>8</v>
-      </c>
-      <c r="D35" t="s">
-        <v>218</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="G35">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>217</v>
-      </c>
-      <c r="B36">
-        <v>8</v>
-      </c>
-      <c r="C36">
-        <v>8</v>
-      </c>
-      <c r="D36" t="s">
-        <v>216</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="G36">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>215</v>
-      </c>
-      <c r="B37">
-        <v>8</v>
-      </c>
-      <c r="C37">
-        <v>6</v>
-      </c>
-      <c r="D37" t="s">
-        <v>214</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>213</v>
-      </c>
-      <c r="B38">
-        <v>8</v>
-      </c>
-      <c r="C38">
-        <v>5</v>
-      </c>
-      <c r="D38" t="s">
-        <v>212</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>211</v>
-      </c>
-      <c r="B39">
-        <v>8</v>
-      </c>
-      <c r="C39">
-        <v>4</v>
-      </c>
-      <c r="D39" t="s">
-        <v>210</v>
-      </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>209</v>
-      </c>
-      <c r="B40">
-        <v>8</v>
-      </c>
-      <c r="C40">
-        <v>2</v>
-      </c>
-      <c r="D40" t="s">
-        <v>208</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>207</v>
-      </c>
-      <c r="B41">
-        <v>8</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41" t="s">
-        <v>206</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>205</v>
-      </c>
-      <c r="B42">
-        <v>8</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="D42" t="s">
-        <v>204</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView topLeftCell="A33" workbookViewId="0">
@@ -3872,11 +3298,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
@@ -4530,4 +3956,1699 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>280</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>278</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>286</v>
+      </c>
+      <c r="G5">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>277</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>276</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>275</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>274</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>273</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>272</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>271</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>270</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>268</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>267</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>266</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>265</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>264</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>263</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>262</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>261</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>260</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>259</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>258</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>257</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>256</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>255</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>254</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>253</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>252</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>251</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>250</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>249</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>248</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>247</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>246</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>245</v>
+      </c>
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>244</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>243</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>242</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>241</v>
+      </c>
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>240</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>239</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>238</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>237</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>236</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>235</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>234</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>233</v>
+      </c>
+      <c r="B28">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>232</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>231</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
+        <v>230</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>229</v>
+      </c>
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>228</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>227</v>
+      </c>
+      <c r="B31">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
+        <v>226</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>225</v>
+      </c>
+      <c r="B32">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>224</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>223</v>
+      </c>
+      <c r="B33">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>222</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>221</v>
+      </c>
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>220</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>219</v>
+      </c>
+      <c r="B35">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>218</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>217</v>
+      </c>
+      <c r="B36">
+        <v>8</v>
+      </c>
+      <c r="C36">
+        <v>8</v>
+      </c>
+      <c r="D36" t="s">
+        <v>216</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>215</v>
+      </c>
+      <c r="B37">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>214</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>213</v>
+      </c>
+      <c r="B38">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>212</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>211</v>
+      </c>
+      <c r="B39">
+        <v>8</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>210</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>209</v>
+      </c>
+      <c r="B40">
+        <v>8</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>208</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>207</v>
+      </c>
+      <c r="B41">
+        <v>8</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>206</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>205</v>
+      </c>
+      <c r="B42">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42" t="s">
+        <v>204</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35:E42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>418</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>417</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>415</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>414</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>413</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="B5" s="8">
+        <v>8</v>
+      </c>
+      <c r="C5" s="8">
+        <v>8</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="8">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>409</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>408</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>407</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>406</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>405</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>404</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>403</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>402</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>401</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>400</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>399</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>398</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>397</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>396</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>395</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>394</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>393</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>392</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>391</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>390</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>389</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>388</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>387</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>386</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>385</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>384</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>383</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>382</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>381</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>380</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>379</v>
+      </c>
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>378</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>377</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>376</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>375</v>
+      </c>
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>374</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>373</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>372</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>371</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>370</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>369</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>368</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>367</v>
+      </c>
+      <c r="B28">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>366</v>
+      </c>
+      <c r="E28" s="7">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>365</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
+        <v>364</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>363</v>
+      </c>
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>362</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>361</v>
+      </c>
+      <c r="B31">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
+        <v>360</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>422</v>
+      </c>
+      <c r="G31">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>359</v>
+      </c>
+      <c r="B32">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>358</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>357</v>
+      </c>
+      <c r="B33">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>356</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>355</v>
+      </c>
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>354</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>353</v>
+      </c>
+      <c r="B35">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <v>5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>352</v>
+      </c>
+      <c r="E35" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>351</v>
+      </c>
+      <c r="B36">
+        <v>8</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>350</v>
+      </c>
+      <c r="E36" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>349</v>
+      </c>
+      <c r="B37">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>348</v>
+      </c>
+      <c r="E37" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>347</v>
+      </c>
+      <c r="B38">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38" t="s">
+        <v>346</v>
+      </c>
+      <c r="E38" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>345</v>
+      </c>
+      <c r="B39">
+        <v>8</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>344</v>
+      </c>
+      <c r="E39" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>343</v>
+      </c>
+      <c r="B40">
+        <v>8</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>342</v>
+      </c>
+      <c r="E40" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>341</v>
+      </c>
+      <c r="B41">
+        <v>8</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>340</v>
+      </c>
+      <c r="E41" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>339</v>
+      </c>
+      <c r="B42">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42" t="s">
+        <v>338</v>
+      </c>
+      <c r="E42" s="7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
929 to 930 batch
</commit_message>
<xml_diff>
--- a/corpus_info.xlsx
+++ b/corpus_info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="460" windowWidth="26020" windowHeight="16920" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="1680" yWindow="480" windowWidth="26020" windowHeight="16920" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="amt_902_096" sheetId="5" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="amt_920_922_tk" sheetId="2" r:id="rId3"/>
     <sheet name="amt_907_915_tk" sheetId="4" r:id="rId4"/>
     <sheet name="amt_923_tk" sheetId="6" r:id="rId5"/>
+    <sheet name="amt_929_tk" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="494">
   <si>
     <t>entryCode</t>
   </si>
@@ -1300,6 +1301,219 @@
   </si>
   <si>
     <t>A good example; sitting pose is very like in a real interview</t>
+  </si>
+  <si>
+    <t>A3CXJ18H14DXBN</t>
+  </si>
+  <si>
+    <t>866945fe96a91e48d993ec72c6038ed3</t>
+  </si>
+  <si>
+    <t>A2NMETDZGRDQ55</t>
+  </si>
+  <si>
+    <t>133e1eedfe840b9dfcb610e14858a136</t>
+  </si>
+  <si>
+    <t>A1C0H8G0YI15MN</t>
+  </si>
+  <si>
+    <t>d3b1ec38087526478e14d653b20ab1e9</t>
+  </si>
+  <si>
+    <t>A2NB54BDTLA0QS</t>
+  </si>
+  <si>
+    <t>036da1d114403dcd4911a56723081951</t>
+  </si>
+  <si>
+    <t>A3MBLDIFREDC5M</t>
+  </si>
+  <si>
+    <t>72c9dfb85f0e65a593a9fc3b4dc11435</t>
+  </si>
+  <si>
+    <t>A2H74STYH3PLT1</t>
+  </si>
+  <si>
+    <t>36de6316630cf172bde72c9242216ed4</t>
+  </si>
+  <si>
+    <t>ADKSME3J8B0PA</t>
+  </si>
+  <si>
+    <t>ff1f954c7711f01be600490f94dfa1f6</t>
+  </si>
+  <si>
+    <t>AMA426ARRZO1O</t>
+  </si>
+  <si>
+    <t>e75be82b2a5ccf056c6654819bc05c87</t>
+  </si>
+  <si>
+    <t>A2DLH5XGBNYXWS</t>
+  </si>
+  <si>
+    <t>e33b1cd62152a988de5c0257c29fdc2d</t>
+  </si>
+  <si>
+    <t>A1IMYG6LYQHOPD</t>
+  </si>
+  <si>
+    <t>d2e71d2029d85d61d6ff06f16b91c6c1</t>
+  </si>
+  <si>
+    <t>A1CE2XPYCDRHVZ</t>
+  </si>
+  <si>
+    <t>cc3d483ba59e741337b189f96ec96d4b</t>
+  </si>
+  <si>
+    <t>A3F832E9XKFRRP</t>
+  </si>
+  <si>
+    <t>b96dece8ee1f8645b6482675b6c653ae</t>
+  </si>
+  <si>
+    <t>A16U1RK5OHN08F</t>
+  </si>
+  <si>
+    <t>b5b6cabacae3055ee30422cdbaaac221</t>
+  </si>
+  <si>
+    <t>A1HBIE5LRTQK1L</t>
+  </si>
+  <si>
+    <t>b0319f326020de32ad3af45b08c55930</t>
+  </si>
+  <si>
+    <t>A220217I0IXYX3</t>
+  </si>
+  <si>
+    <t>a6d4ad452fde42bcaff7286a0477024f</t>
+  </si>
+  <si>
+    <t>A1OBB3PWYWK9KK</t>
+  </si>
+  <si>
+    <t>9e8886135ca79ca16b880f944fa69acc</t>
+  </si>
+  <si>
+    <t>8956e6c21c8cc34b0745eb4f3151ce4f</t>
+  </si>
+  <si>
+    <t>A3QXV94C2J0LQ</t>
+  </si>
+  <si>
+    <t>88fd91371fcf76200f68a615f4a359de</t>
+  </si>
+  <si>
+    <t>A2GZ0MWS800M6R</t>
+  </si>
+  <si>
+    <t>798785112a4b2872e4ae00fb6b1eec2f</t>
+  </si>
+  <si>
+    <t>AV08UM669CO02</t>
+  </si>
+  <si>
+    <t>63ee40e6f5823c5076e408eafec13701</t>
+  </si>
+  <si>
+    <t>A1G4ZQ8NAB94TT</t>
+  </si>
+  <si>
+    <t>625878bbe7175a773b52b1e66b1d2105</t>
+  </si>
+  <si>
+    <t>AOLLFPCWXJVA6</t>
+  </si>
+  <si>
+    <t>61137aa97a7daefe8c0b5b7a6e7e66c7</t>
+  </si>
+  <si>
+    <t>A1DUH3RLI00YQM</t>
+  </si>
+  <si>
+    <t>5f697dbe33cc16a5676ae1956d0f86aa</t>
+  </si>
+  <si>
+    <t>A2ZLDAQZIN5WZC</t>
+  </si>
+  <si>
+    <t>5f59e63618bb40a726c83a1da9fabcf4</t>
+  </si>
+  <si>
+    <t>A2C4271VBZQCR7</t>
+  </si>
+  <si>
+    <t>5bbd81263d7ac05504e0dd0e3279b79c</t>
+  </si>
+  <si>
+    <t>A1FHBPFI2UNASX</t>
+  </si>
+  <si>
+    <t>4a47c45e5d5f36706ebec7a4f163c9a8</t>
+  </si>
+  <si>
+    <t>A1XB03X4J35ATE</t>
+  </si>
+  <si>
+    <t>49bf7822e28fc4244ff4b480647bbc27</t>
+  </si>
+  <si>
+    <t>A39NKZDUFD70NV</t>
+  </si>
+  <si>
+    <t>462343b842422e8203c07aa7c24b86a9</t>
+  </si>
+  <si>
+    <t>A3LUXDAIWTYTZL</t>
+  </si>
+  <si>
+    <t>433cee823dc7f7e921a5096abab454b0</t>
+  </si>
+  <si>
+    <t>A2809ZZ59YT4C0</t>
+  </si>
+  <si>
+    <t>3ddc21c75fa5950646a46a99416ab3a7</t>
+  </si>
+  <si>
+    <t>A1QDWIDKBZK759</t>
+  </si>
+  <si>
+    <t>3cca3f67f9aff39473637c4ca1b3b8f4</t>
+  </si>
+  <si>
+    <t>AK7LGB1QOGA1P</t>
+  </si>
+  <si>
+    <t>342e7519b04c94956408b39a8300e1c2</t>
+  </si>
+  <si>
+    <t>A4ZW4GNQ98HV6</t>
+  </si>
+  <si>
+    <t>3129db589e16da52605c903eac08e2af</t>
+  </si>
+  <si>
+    <t>A2PE32I58ANCDD</t>
+  </si>
+  <si>
+    <t>20a55ea9098263a79f5eacbd2e93e3c9</t>
+  </si>
+  <si>
+    <t>A2J9S68Y0ROJ8W</t>
+  </si>
+  <si>
+    <t>1808b557f62e5112da80067517465799</t>
+  </si>
+  <si>
+    <t>video playing is choppy</t>
+  </si>
+  <si>
+    <t>camera has not been started</t>
   </si>
 </sst>
 </file>
@@ -4812,8 +5026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35:E42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5651,4 +5865,732 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="36.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>491</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>490</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>489</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>488</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>487</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>486</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>484</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>483</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>482</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>481</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>480</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>479</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>478</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>477</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>476</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>475</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>474</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>473</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>472</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>471</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>470</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>469</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>468</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>467</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>466</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>465</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>464</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>463</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>462</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>461</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>460</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>459</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>458</v>
+      </c>
+      <c r="E18" s="7">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>457</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>456</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>455</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>101</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>453</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>452</v>
+      </c>
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>451</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>450</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>449</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>448</v>
+      </c>
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>447</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>446</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>445</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>444</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>443</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>442</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>441</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>440</v>
+      </c>
+      <c r="B28">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>439</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>438</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
+        <v>437</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>436</v>
+      </c>
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>435</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>434</v>
+      </c>
+      <c r="B31">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>7</v>
+      </c>
+      <c r="D31" t="s">
+        <v>433</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>432</v>
+      </c>
+      <c r="B32">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>431</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>430</v>
+      </c>
+      <c r="B33">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>429</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>428</v>
+      </c>
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34" t="s">
+        <v>427</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>426</v>
+      </c>
+      <c r="B35">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>425</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>424</v>
+      </c>
+      <c r="B36">
+        <v>8</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>423</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
HIT 10/4 to 10/7
</commit_message>
<xml_diff>
--- a/corpus_info.xlsx
+++ b/corpus_info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="480" windowWidth="26020" windowHeight="16920" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="1680" yWindow="480" windowWidth="26020" windowHeight="16920" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="amt_902_096" sheetId="5" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="amt_907_915_tk" sheetId="4" r:id="rId4"/>
     <sheet name="amt_923_tk" sheetId="6" r:id="rId5"/>
     <sheet name="amt_929_tk" sheetId="7" r:id="rId6"/>
+    <sheet name="amt_104_tk" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="598">
   <si>
     <t>entryCode</t>
   </si>
@@ -1514,6 +1515,318 @@
   </si>
   <si>
     <t>camera has not been started</t>
+  </si>
+  <si>
+    <t>0449e1ec3a904f407b0a7d2f4c9c0c79</t>
+  </si>
+  <si>
+    <t>A36D0LIE5AKL2P</t>
+  </si>
+  <si>
+    <t>0d315e83d7930f9833a05911063d34a9</t>
+  </si>
+  <si>
+    <t>A3T111ZNMZ7A5D</t>
+  </si>
+  <si>
+    <t>0f2c9354f74342a454c4cf9f7e49963f</t>
+  </si>
+  <si>
+    <t>A2ZGQUSBB0TMK4</t>
+  </si>
+  <si>
+    <t>19dd3ea9be71bfae5cc727811e99d17c</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AUGR3YWEMVIY7</t>
+  </si>
+  <si>
+    <t>1af3743c21839da61d181cbb5803c340</t>
+  </si>
+  <si>
+    <t>A1D0JL4MJ7XSGV</t>
+  </si>
+  <si>
+    <t>1d5ff8280452bb27571b08f5927b56d4</t>
+  </si>
+  <si>
+    <t>A330ISTI9O9WTI</t>
+  </si>
+  <si>
+    <t>28e1ee5d09ef573b627af22c47ad6f63</t>
+  </si>
+  <si>
+    <t>A1ZB2NY0F9QNP0</t>
+  </si>
+  <si>
+    <t>2b5326c191e10fcddecf9f7fb478bbc7</t>
+  </si>
+  <si>
+    <t>A1WR6M74EOTJNY</t>
+  </si>
+  <si>
+    <t>2c2da194a6086709c458ebb5097e45e2</t>
+  </si>
+  <si>
+    <t>AR72L0JX4D03W</t>
+  </si>
+  <si>
+    <t>2e433b6fa7238ec15676dc3269081849</t>
+  </si>
+  <si>
+    <t>A2JLSY93R8P8DS</t>
+  </si>
+  <si>
+    <t>339bffeb4ebd89494888374822683baa</t>
+  </si>
+  <si>
+    <t>A325BIJIG3AK1T</t>
+  </si>
+  <si>
+    <t>3970d2c3503b521357dc741561c86220</t>
+  </si>
+  <si>
+    <t>A121W3A5FW3MD4</t>
+  </si>
+  <si>
+    <t>39def480018ef9bb07a1d8664f7e1257</t>
+  </si>
+  <si>
+    <t>3e084d125ad51c6de592f93d7540c59b</t>
+  </si>
+  <si>
+    <t>A3PGUPNMOU5BPW</t>
+  </si>
+  <si>
+    <t>41ae951683f8a81bd4c3d7d1e1e57547</t>
+  </si>
+  <si>
+    <t>A3RIFUEQ95MR16</t>
+  </si>
+  <si>
+    <t>5522cc12c09f2469f7cc856bc0159aaf</t>
+  </si>
+  <si>
+    <t>A1GOJEDZM2CQTN</t>
+  </si>
+  <si>
+    <t>5dd3e271ccd3b8d7f3e3f47985bfada9</t>
+  </si>
+  <si>
+    <t>A3FC1KVPO4RGIN</t>
+  </si>
+  <si>
+    <t>5e353316e8373543cd2e041c303bda16</t>
+  </si>
+  <si>
+    <t>A9UCDP0W2FVAV</t>
+  </si>
+  <si>
+    <t>6c516879d637b6746ce52c55af5cf5cc</t>
+  </si>
+  <si>
+    <t>716367eb320d1ee182e190690a93a8e0</t>
+  </si>
+  <si>
+    <t>A2ISX4NLTUMNPD</t>
+  </si>
+  <si>
+    <t>7fa1bd5284f4c08135070397228f9bb9</t>
+  </si>
+  <si>
+    <t>A2YV50DPZCX2JN</t>
+  </si>
+  <si>
+    <t>8515d632856d816e8e5d3ec96f929877</t>
+  </si>
+  <si>
+    <t>A1YGENVE7OI5JL</t>
+  </si>
+  <si>
+    <t>85d1efe45a2b7ab2c0f9a592e9673dfa</t>
+  </si>
+  <si>
+    <t>ASX5NVC2MTJ3B</t>
+  </si>
+  <si>
+    <t>884cd6903eb684d67ebb4ef3f5e54e22</t>
+  </si>
+  <si>
+    <t>A2UCSSENYIMEIW</t>
+  </si>
+  <si>
+    <t>89e9f1b038cf56a572049c20e6fe598a</t>
+  </si>
+  <si>
+    <t>A36A8J9M8GSIYF</t>
+  </si>
+  <si>
+    <t>8d411380268b2935eeec299b479df8d5</t>
+  </si>
+  <si>
+    <t>A3TZTSRQJQ97L8</t>
+  </si>
+  <si>
+    <t>8e8d7bd42c782f1a84b97b80bec7433f</t>
+  </si>
+  <si>
+    <t>A37EV8RZ82WT8E</t>
+  </si>
+  <si>
+    <t>9232a51f2edc9a32d8eeb8f93e6e8a63</t>
+  </si>
+  <si>
+    <t>AAYRVW54BRE8R</t>
+  </si>
+  <si>
+    <t>9469fada413f26e0131e366202714c94</t>
+  </si>
+  <si>
+    <t>A2JQ7V9EWJ51T2</t>
+  </si>
+  <si>
+    <t>9f8a8ef97677f66537e0d99bb2478f48</t>
+  </si>
+  <si>
+    <t>AQCWC087K8YCR</t>
+  </si>
+  <si>
+    <t>a14058177bdb2089e226ef337b8bda36</t>
+  </si>
+  <si>
+    <t>A29X709ZWO05H2</t>
+  </si>
+  <si>
+    <t>a3f5c6f6bb44cbbb1e5fd97413ca2f50</t>
+  </si>
+  <si>
+    <t>A3DH2RU1CFTXAP</t>
+  </si>
+  <si>
+    <t>adc04da710e33abdd62c8ec395a15e34</t>
+  </si>
+  <si>
+    <t>AR5E0ZVWKJA95</t>
+  </si>
+  <si>
+    <t>b1764000277fa055127df47c84b72dab</t>
+  </si>
+  <si>
+    <t>b682b80e30156e2304d4bd92ce8c563e</t>
+  </si>
+  <si>
+    <t>A2EBQ6NGXSXRW0</t>
+  </si>
+  <si>
+    <t>b8b503c7a8bbbecc84c8e448a05cefcb</t>
+  </si>
+  <si>
+    <t>A1CTOT46Y4W11J</t>
+  </si>
+  <si>
+    <t>c1500ef2b6fe0b3a83a5a598d8c2310f</t>
+  </si>
+  <si>
+    <t>d4e7a8b9d1e10a53d6cab0d4c50850e9</t>
+  </si>
+  <si>
+    <t>A1TISWAW29WUGA</t>
+  </si>
+  <si>
+    <t>d93e74eae15c4983f5ffb43b45febf03</t>
+  </si>
+  <si>
+    <t>A2OR95QZT4H80T</t>
+  </si>
+  <si>
+    <t>d9579a69358f7e16c65e60ba08e14201</t>
+  </si>
+  <si>
+    <t>A34W8AC87LAAS</t>
+  </si>
+  <si>
+    <t>de56fac608c314d8c1c5370d63df0a7b</t>
+  </si>
+  <si>
+    <t>A1QG4N21BF61PC</t>
+  </si>
+  <si>
+    <t>de5d1b5a878c07c5e8d3f43cbedcf2c8</t>
+  </si>
+  <si>
+    <t>e256153fbe35829495511810e3dc96ff</t>
+  </si>
+  <si>
+    <t>A5NKVJX6QEXEY</t>
+  </si>
+  <si>
+    <t>effc4b0420cb5df36b01e4954372d2cd</t>
+  </si>
+  <si>
+    <t>A2VBSFSJXLZZ7A</t>
+  </si>
+  <si>
+    <t>f5148d89f7857408575204c24bb12714</t>
+  </si>
+  <si>
+    <t>ALF9AAZGQP4K5</t>
+  </si>
+  <si>
+    <t>ffb621477e000af8f66717bcd6278482</t>
+  </si>
+  <si>
+    <t>A60BX1JSJRYAX</t>
+  </si>
+  <si>
+    <t>e3809ec34cf9f345ed4e59ab033f9db3</t>
+  </si>
+  <si>
+    <t>A260QC80Q9VX7Z</t>
+  </si>
+  <si>
+    <t>7d5799f278b55122c8de5542180d43ab</t>
+  </si>
+  <si>
+    <t>A194E79BDFEZIU</t>
+  </si>
+  <si>
+    <t>8a530de58927745c927fc8ff752d0ee6</t>
+  </si>
+  <si>
+    <t>A37H5799TLDXUT</t>
+  </si>
+  <si>
+    <t>de82a643ed658b40447cfcb85249956e</t>
+  </si>
+  <si>
+    <t>A2FV527DH1S2Y7</t>
+  </si>
+  <si>
+    <t>85da6399de4f8791b7e5f4a36d81fbc7</t>
+  </si>
+  <si>
+    <t>A2WCV7ULUPKVNQ</t>
+  </si>
+  <si>
+    <t>3f10bb3b932ba8b6f95fffd18b69dbc1</t>
+  </si>
+  <si>
+    <t>A1S8DYWNS59XWB</t>
+  </si>
+  <si>
+    <t>Sound is choppy for video 8</t>
+  </si>
+  <si>
+    <t>sound is choppy for video 1 to 4</t>
+  </si>
+  <si>
+    <t>video quality is poor.</t>
+  </si>
+  <si>
+    <t>web cam is too old. Just got very small videos</t>
+  </si>
+  <si>
+    <t>partial face</t>
   </si>
 </sst>
 </file>
@@ -5871,7 +6184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -6593,4 +6906,1076 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48:F53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.5" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="6" max="6" width="40" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>494</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>495</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>496</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>497</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>498</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>499</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>500</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>501</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>502</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>503</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>504</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>505</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>506</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>507</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>508</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>509</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>510</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>511</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>513</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>514</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>515</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>516</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>517</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>518</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>486</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>519</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>520</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>521</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>522</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>523</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>524</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>525</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>526</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>528</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>529</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>149</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>530</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>531</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>532</v>
+      </c>
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>533</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>534</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>535</v>
+      </c>
+      <c r="E23" s="7">
+        <v>0</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>536</v>
+      </c>
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>537</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>538</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>539</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>540</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>541</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>542</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>543</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>544</v>
+      </c>
+      <c r="B28">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>545</v>
+      </c>
+      <c r="E28" s="7">
+        <v>0</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>546</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
+        <v>547</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>548</v>
+      </c>
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>549</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>550</v>
+      </c>
+      <c r="B31">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
+        <v>551</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>552</v>
+      </c>
+      <c r="B32">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>553</v>
+      </c>
+      <c r="E32" s="7">
+        <v>0</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>554</v>
+      </c>
+      <c r="B33">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>555</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>556</v>
+      </c>
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>557</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>558</v>
+      </c>
+      <c r="B35">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>559</v>
+      </c>
+      <c r="B36">
+        <v>8</v>
+      </c>
+      <c r="C36">
+        <v>8</v>
+      </c>
+      <c r="D36" t="s">
+        <v>560</v>
+      </c>
+      <c r="E36" s="7">
+        <v>0</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>561</v>
+      </c>
+      <c r="B37">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>8</v>
+      </c>
+      <c r="D37" t="s">
+        <v>562</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>563</v>
+      </c>
+      <c r="B38">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>8</v>
+      </c>
+      <c r="D38" t="s">
+        <v>191</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>564</v>
+      </c>
+      <c r="B39">
+        <v>8</v>
+      </c>
+      <c r="C39">
+        <v>8</v>
+      </c>
+      <c r="D39" t="s">
+        <v>565</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>566</v>
+      </c>
+      <c r="B40">
+        <v>8</v>
+      </c>
+      <c r="C40">
+        <v>8</v>
+      </c>
+      <c r="D40" t="s">
+        <v>567</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>568</v>
+      </c>
+      <c r="B41">
+        <v>8</v>
+      </c>
+      <c r="C41">
+        <v>8</v>
+      </c>
+      <c r="D41" t="s">
+        <v>569</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>570</v>
+      </c>
+      <c r="B42">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>8</v>
+      </c>
+      <c r="D42" t="s">
+        <v>571</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>572</v>
+      </c>
+      <c r="B43">
+        <v>8</v>
+      </c>
+      <c r="C43">
+        <v>8</v>
+      </c>
+      <c r="D43" t="s">
+        <v>167</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>573</v>
+      </c>
+      <c r="B44">
+        <v>8</v>
+      </c>
+      <c r="C44">
+        <v>8</v>
+      </c>
+      <c r="D44" t="s">
+        <v>574</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>575</v>
+      </c>
+      <c r="B45">
+        <v>8</v>
+      </c>
+      <c r="C45">
+        <v>8</v>
+      </c>
+      <c r="D45" t="s">
+        <v>576</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>577</v>
+      </c>
+      <c r="B46">
+        <v>8</v>
+      </c>
+      <c r="C46">
+        <v>8</v>
+      </c>
+      <c r="D46" t="s">
+        <v>578</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>579</v>
+      </c>
+      <c r="B47">
+        <v>8</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+      <c r="D47" t="s">
+        <v>580</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="G47">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>581</v>
+      </c>
+      <c r="B48">
+        <v>8</v>
+      </c>
+      <c r="C48">
+        <v>7</v>
+      </c>
+      <c r="D48" t="s">
+        <v>582</v>
+      </c>
+      <c r="E48" s="7">
+        <v>0</v>
+      </c>
+      <c r="F48" s="7"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>583</v>
+      </c>
+      <c r="B49">
+        <v>8</v>
+      </c>
+      <c r="C49">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s">
+        <v>584</v>
+      </c>
+      <c r="E49" s="7">
+        <v>0</v>
+      </c>
+      <c r="F49" s="7"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>585</v>
+      </c>
+      <c r="B50">
+        <v>8</v>
+      </c>
+      <c r="C50">
+        <v>6</v>
+      </c>
+      <c r="D50" t="s">
+        <v>586</v>
+      </c>
+      <c r="E50" s="7">
+        <v>0</v>
+      </c>
+      <c r="F50" s="7"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>587</v>
+      </c>
+      <c r="B51">
+        <v>8</v>
+      </c>
+      <c r="C51">
+        <v>6</v>
+      </c>
+      <c r="D51" t="s">
+        <v>588</v>
+      </c>
+      <c r="E51" s="7">
+        <v>0</v>
+      </c>
+      <c r="F51" s="7"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>589</v>
+      </c>
+      <c r="B52">
+        <v>8</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s">
+        <v>590</v>
+      </c>
+      <c r="E52" s="7">
+        <v>0</v>
+      </c>
+      <c r="F52" s="7"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>591</v>
+      </c>
+      <c r="B53">
+        <v>8</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53" t="s">
+        <v>592</v>
+      </c>
+      <c r="E53" s="7">
+        <v>0</v>
+      </c>
+      <c r="F53" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
HIT 10/7 to 10/10
</commit_message>
<xml_diff>
--- a/corpus_info.xlsx
+++ b/corpus_info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="480" windowWidth="26020" windowHeight="16920" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="1460" yWindow="460" windowWidth="26020" windowHeight="16920" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="amt_902_096" sheetId="5" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="amt_923_tk" sheetId="6" r:id="rId5"/>
     <sheet name="amt_929_tk" sheetId="7" r:id="rId6"/>
     <sheet name="amt_104_tk" sheetId="8" r:id="rId7"/>
+    <sheet name="amt_107_tk" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="646">
   <si>
     <t>entryCode</t>
   </si>
@@ -1827,6 +1828,150 @@
   </si>
   <si>
     <t>partial face</t>
+  </si>
+  <si>
+    <t>07c1b49fc36c83ed147b5d4806d62728</t>
+  </si>
+  <si>
+    <t>A1U6P62U5C8XDF</t>
+  </si>
+  <si>
+    <t>0a12b3d1b8e74617986b01bb61119a20</t>
+  </si>
+  <si>
+    <t>A10V3PXHLR4VRM</t>
+  </si>
+  <si>
+    <t>0c92a8a38b012853773e5891b32100c2</t>
+  </si>
+  <si>
+    <t>ASN25PIODXIPJ</t>
+  </si>
+  <si>
+    <t>3e7f5290edb5285f43e51ee43bd43631</t>
+  </si>
+  <si>
+    <t>A15Y215D57OSO5</t>
+  </si>
+  <si>
+    <t>404b43147fe589cb92e0e93ea8c470f8</t>
+  </si>
+  <si>
+    <t>A1S77Y96MFAY5F</t>
+  </si>
+  <si>
+    <t>4395b5fe20328e109000bebd244159d7</t>
+  </si>
+  <si>
+    <t>A3J34I6O9MYJI9</t>
+  </si>
+  <si>
+    <t>447764ae1ebaa5fcd17fab9bae8bfb15</t>
+  </si>
+  <si>
+    <t>A2UQI9BEX18NCQ</t>
+  </si>
+  <si>
+    <t>4dd9c253aa8a5b7e6fc83ac01dab6097</t>
+  </si>
+  <si>
+    <t>A2Q2IMR3GBBTU3</t>
+  </si>
+  <si>
+    <t>7eaf9d98c07e6484c70e21098c5df31d</t>
+  </si>
+  <si>
+    <t>A4WYG70EHTB4G</t>
+  </si>
+  <si>
+    <t>905f92209e8b6b9d64f93901148c1a14</t>
+  </si>
+  <si>
+    <t>A20HZD952T4B2O</t>
+  </si>
+  <si>
+    <t>a5a80517c6bfc58c53683c27ec1b7965</t>
+  </si>
+  <si>
+    <t>ABO6TXB8QJ3U8</t>
+  </si>
+  <si>
+    <t>a6579df0dc04c86c6b98fd51aad4b053</t>
+  </si>
+  <si>
+    <t>A1F1OZ54G177D8</t>
+  </si>
+  <si>
+    <t>a6bef7b4c0dc998731d7ad95d2909ccf</t>
+  </si>
+  <si>
+    <t>b02017004f31bc730099d4b897947a2b</t>
+  </si>
+  <si>
+    <t>A3ELLEKJ287JZZ</t>
+  </si>
+  <si>
+    <t>ba8332bddf8544abcc3f3dd2793e950d</t>
+  </si>
+  <si>
+    <t>A24MFJ893DQKW1</t>
+  </si>
+  <si>
+    <t>cd9566a048e5480ca1071e5fe6ce33f2</t>
+  </si>
+  <si>
+    <t>d6c8e5d2d0cc1db85a8370e95ebf4276</t>
+  </si>
+  <si>
+    <t>A2MNKVHVCZLJ79</t>
+  </si>
+  <si>
+    <t>d8cf9bf5aad89a5a4ba0e3977dd53bac</t>
+  </si>
+  <si>
+    <t>A1PT3FU3M6KN2R</t>
+  </si>
+  <si>
+    <t>daf725dc00c58bef02478a179d0fb412</t>
+  </si>
+  <si>
+    <t>A31XVMN754ZGGA</t>
+  </si>
+  <si>
+    <t>db5fc8711a9efe909bbfe6470bcaa186</t>
+  </si>
+  <si>
+    <t>A1VBQK9HNTBJL4</t>
+  </si>
+  <si>
+    <t>de86047abe8b9d3f0fe4b19bed45127c</t>
+  </si>
+  <si>
+    <t>A2581F7TDPAMBQ</t>
+  </si>
+  <si>
+    <t>f434e5e3e6bc045dfddb956e5183a024</t>
+  </si>
+  <si>
+    <t>A2FIYSZS8BSHCB</t>
+  </si>
+  <si>
+    <t>d38169217f802e742f0de15264cfbb49</t>
+  </si>
+  <si>
+    <t>A3S3MPBFR9A0LJ</t>
+  </si>
+  <si>
+    <t>repeated turker; watching TV while answering</t>
+  </si>
+  <si>
+    <t>saturated face, esp. glasses</t>
+  </si>
+  <si>
+    <t>mouth was covered</t>
+  </si>
+  <si>
+    <t>repeated turker</t>
   </si>
 </sst>
 </file>
@@ -2593,7 +2738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -3830,7 +3975,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6185,7 +6330,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E1" sqref="E1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6912,8 +7057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48:F53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7978,4 +8123,524 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="36.5" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="6" max="6" width="37.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>598</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>599</v>
+      </c>
+      <c r="E2" s="8">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>600</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>601</v>
+      </c>
+      <c r="E3" s="8">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>602</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>603</v>
+      </c>
+      <c r="E4" s="8">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>604</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>605</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>606</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>607</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>608</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>609</v>
+      </c>
+      <c r="E7" s="8">
+        <v>1</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>610</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>611</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>612</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>613</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>614</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>615</v>
+      </c>
+      <c r="E10" s="8">
+        <v>1</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="G10">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>616</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>617</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>618</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>619</v>
+      </c>
+      <c r="E12" s="8">
+        <v>1</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>620</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>621</v>
+      </c>
+      <c r="E13" s="8">
+        <v>1</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>622</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>389</v>
+      </c>
+      <c r="E14" s="8">
+        <v>1</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>623</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>624</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>625</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>626</v>
+      </c>
+      <c r="E16" s="8">
+        <v>1</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>627</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>628</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>629</v>
+      </c>
+      <c r="E18" s="8">
+        <v>0</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>630</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>631</v>
+      </c>
+      <c r="E19" s="8">
+        <v>1</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>632</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>633</v>
+      </c>
+      <c r="E20" s="8">
+        <v>1</v>
+      </c>
+      <c r="F20" s="8"/>
+      <c r="G20">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>634</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>635</v>
+      </c>
+      <c r="E21" s="8">
+        <v>1</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>636</v>
+      </c>
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>637</v>
+      </c>
+      <c r="E22" s="8">
+        <v>1</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>638</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>639</v>
+      </c>
+      <c r="E23" s="8">
+        <v>0</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>640</v>
+      </c>
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>641</v>
+      </c>
+      <c r="E24" s="8">
+        <v>0</v>
+      </c>
+      <c r="F24" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
HIT 1010 to 1013
- finished the last HIT
- turker # now 255.
</commit_message>
<xml_diff>
--- a/corpus_info.xlsx
+++ b/corpus_info.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="460" windowWidth="26020" windowHeight="16920" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="2260" yWindow="460" windowWidth="26020" windowHeight="16920" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="amt_902_096" sheetId="5" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="amt_929_tk" sheetId="7" r:id="rId6"/>
     <sheet name="amt_104_tk" sheetId="8" r:id="rId7"/>
     <sheet name="amt_107_tk" sheetId="9" r:id="rId8"/>
+    <sheet name="amt_1010_tk" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="703">
   <si>
     <t>entryCode</t>
   </si>
@@ -1972,13 +1973,184 @@
   </si>
   <si>
     <t>repeated turker</t>
+  </si>
+  <si>
+    <t>0303b492950488f5ced94764cd145f1b</t>
+  </si>
+  <si>
+    <t>A2WW3LCEVWB332</t>
+  </si>
+  <si>
+    <t>09a23d54ada60b7ce9c3f3b95428b57e</t>
+  </si>
+  <si>
+    <t>A1P1X1QY3N0NK7</t>
+  </si>
+  <si>
+    <t>1278317ac7fd2d360c79f1b18039877d</t>
+  </si>
+  <si>
+    <t>A3HNAJE7OJP66A</t>
+  </si>
+  <si>
+    <t>2414528a0dc3da14f4b315e8926804ce</t>
+  </si>
+  <si>
+    <t>A351VRNE012LLG</t>
+  </si>
+  <si>
+    <t>44f2d11c3b2588e2f7a9eacee89c0a01</t>
+  </si>
+  <si>
+    <t>A2VP9870OO2MPH</t>
+  </si>
+  <si>
+    <t>501c4263219198766a2bd57e8f935760</t>
+  </si>
+  <si>
+    <t>A2BO72OE2W8OGI</t>
+  </si>
+  <si>
+    <t>5d40f37dcf1efe145de65ccb9f5b65e8</t>
+  </si>
+  <si>
+    <t>A3AK905WEI3PMV</t>
+  </si>
+  <si>
+    <t>6dd7a015fe077150318eb3b4fb5ac222</t>
+  </si>
+  <si>
+    <t>A2NR1NLG4HBU9K</t>
+  </si>
+  <si>
+    <t>84c055438d48fcd87b9e1bd9bde2abee</t>
+  </si>
+  <si>
+    <t>A29SLP0FSTR2AY</t>
+  </si>
+  <si>
+    <t>88df45824fc58d2ee84aaabb3491b084</t>
+  </si>
+  <si>
+    <t>A3MELYYGRJ61SX</t>
+  </si>
+  <si>
+    <t>925def94d0a958778dea058a2c8b0420</t>
+  </si>
+  <si>
+    <t>A3EHFFBEFICG9D</t>
+  </si>
+  <si>
+    <t>a7f4bbdec3c9680358b4ae861e048d5b</t>
+  </si>
+  <si>
+    <t>AL9JECXO2GD79</t>
+  </si>
+  <si>
+    <t>af70f3d3a4a1566e3c1e7e96d2e5bc5b</t>
+  </si>
+  <si>
+    <t>A31MS4JN47HSAM</t>
+  </si>
+  <si>
+    <t>b7e273b4adf45c0eb65a5ab05c9ab530</t>
+  </si>
+  <si>
+    <t>cc0a1f42b976f0ba9109dafa31cc1884</t>
+  </si>
+  <si>
+    <t>A2AXXK0K20IO1Z</t>
+  </si>
+  <si>
+    <t>d25d57f6dd0dabf681e1e1784fe57b1f</t>
+  </si>
+  <si>
+    <t>A1YBGCRZYYJK0S</t>
+  </si>
+  <si>
+    <t>d4c7a9ed42400055ec83cb90a064c12d</t>
+  </si>
+  <si>
+    <t>A1ZI4NP3NGHH9D</t>
+  </si>
+  <si>
+    <t>db233d26d57b90e3364dadc8025b73db</t>
+  </si>
+  <si>
+    <t>A24LP60QLUKQWX</t>
+  </si>
+  <si>
+    <t>dcfe8b1679f61eaca23bad4e84732b8a</t>
+  </si>
+  <si>
+    <t>A2UPZSAKT77V3L</t>
+  </si>
+  <si>
+    <t>e2e518c5d577dae172ca9320067676c9</t>
+  </si>
+  <si>
+    <t>AJMWTFJTL8RLM</t>
+  </si>
+  <si>
+    <t>e7b350da0354f00e9fb277d567671536</t>
+  </si>
+  <si>
+    <t>A2COQ07WP2OBGD</t>
+  </si>
+  <si>
+    <t>e8500b7570b24737c7239e419ae3c84f</t>
+  </si>
+  <si>
+    <t>A3IGKAGURMDJAG</t>
+  </si>
+  <si>
+    <t>ebecbc9e20e6f599dc34bb0a11da5049</t>
+  </si>
+  <si>
+    <t>A1GUL845MKMPK7</t>
+  </si>
+  <si>
+    <t>f0d94039a3016860ec8ab6cb80c2de51</t>
+  </si>
+  <si>
+    <t>AA7ALKNSH0WYB</t>
+  </si>
+  <si>
+    <t>f52ea6c92544d1d2076c7365f323e0ff</t>
+  </si>
+  <si>
+    <t>A3TQ04VI76IEMC</t>
+  </si>
+  <si>
+    <t>93140c3c038b9e3cb7d42485f394d65c</t>
+  </si>
+  <si>
+    <t>a3aac525523a0c1bd81d570ba914715e</t>
+  </si>
+  <si>
+    <t>A3I5AIHW1HI3F1</t>
+  </si>
+  <si>
+    <t>f8900d61a2d30bc04c10b1f54d396163</t>
+  </si>
+  <si>
+    <t>AK4W742U46WN5</t>
+  </si>
+  <si>
+    <t>audio issue</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>some videos cannot be played</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2010,6 +2182,14 @@
     <font>
       <sz val="12"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2050,7 +2230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2061,6 +2241,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6330,7 +6511,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8129,8 +8310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8643,4 +8824,608 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.83203125" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>646</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>647</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>648</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>649</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>650</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>651</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>652</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>653</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>654</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>655</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>656</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>657</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>658</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>659</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>660</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>661</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>662</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>663</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>664</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>665</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>666</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>667</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>668</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>669</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>670</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>671</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>672</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>673</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>674</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>675</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>676</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>677</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>678</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>679</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>680</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>681</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>682</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>683</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>684</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>685</v>
+      </c>
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>686</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>687</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>688</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>689</v>
+      </c>
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>690</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>691</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>692</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="G25" s="10">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>693</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>694</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>695</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>696</v>
+      </c>
+      <c r="B28">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>697</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>698</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>699</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>702</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
HIT 1014 to 1017
</commit_message>
<xml_diff>
--- a/corpus_info.xlsx
+++ b/corpus_info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="460" windowWidth="26020" windowHeight="16920" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="2260" yWindow="460" windowWidth="26020" windowHeight="16920" tabRatio="500" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="amt_902_096" sheetId="5" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="amt_104_tk" sheetId="8" r:id="rId7"/>
     <sheet name="amt_107_tk" sheetId="9" r:id="rId8"/>
     <sheet name="amt_1010_tk" sheetId="10" r:id="rId9"/>
+    <sheet name="amt_1014_tk" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="703">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="714">
   <si>
     <t>entryCode</t>
   </si>
@@ -2144,6 +2145,39 @@
   </si>
   <si>
     <t>some videos cannot be played</t>
+  </si>
+  <si>
+    <t>037a85c1d1ff323db8dccda5fa870e8f</t>
+  </si>
+  <si>
+    <t>AT5ZQMI28TZ7J</t>
+  </si>
+  <si>
+    <t>1c56ff1826cfb0ecfc1bfdcaa7cfad40</t>
+  </si>
+  <si>
+    <t>442e0c115a4f4f6a33f7d49b640b6102</t>
+  </si>
+  <si>
+    <t>AVV2YBK3KUPFV</t>
+  </si>
+  <si>
+    <t>adfd153ed532ff0f96cb3d61e8dfd939</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A2FV527DH1S2Y7</t>
+  </si>
+  <si>
+    <t>de4cfeb603d6817e29e3c084bfaaafb8</t>
+  </si>
+  <si>
+    <t>fbf3f3051efbbf3ee4644d4b833a86a8</t>
+  </si>
+  <si>
+    <t>A110JBKYAC0WAW</t>
+  </si>
+  <si>
+    <t>didn't answer questions</t>
   </si>
 </sst>
 </file>
@@ -2915,6 +2949,169 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.83203125" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>703</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>704</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>705</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>706</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>707</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>708</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>709</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>710</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>232</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>711</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>712</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>260</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G62"/>
@@ -8830,8 +9027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>